<commit_message>
Added all the ICs and made a fix on the line 37 which counts the number of ICs
</commit_message>
<xml_diff>
--- a/ic_tester/data/embedded_sysetms_ICS_readings.xlsx
+++ b/ic_tester/data/embedded_sysetms_ICS_readings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\embedded_project\ic_tester\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3F0CB18-96B8-4921-B5FF-5C935CE72BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF961509-188D-48FA-B69B-C7F8C123CCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{6CF21B77-D1EF-4F55-A096-EC4EA1282863}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="196">
   <si>
     <t>G1</t>
   </si>
@@ -477,6 +477,153 @@
   </si>
   <si>
     <t>Q9</t>
+  </si>
+  <si>
+    <t>8585AH</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>RESET OUT</t>
+  </si>
+  <si>
+    <t>SDD</t>
+  </si>
+  <si>
+    <t>SID</t>
+  </si>
+  <si>
+    <t>TRAP</t>
+  </si>
+  <si>
+    <t>RST 7.5</t>
+  </si>
+  <si>
+    <t>RST 6.5</t>
+  </si>
+  <si>
+    <t>RST 5.5</t>
+  </si>
+  <si>
+    <t>INTA</t>
+  </si>
+  <si>
+    <t>AD0</t>
+  </si>
+  <si>
+    <t>AD1</t>
+  </si>
+  <si>
+    <t>AD2</t>
+  </si>
+  <si>
+    <t>AD3</t>
+  </si>
+  <si>
+    <t>AD4</t>
+  </si>
+  <si>
+    <t>AD5</t>
+  </si>
+  <si>
+    <t>AD6</t>
+  </si>
+  <si>
+    <t>AD7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>S0</t>
+  </si>
+  <si>
+    <t>ALE</t>
+  </si>
+  <si>
+    <t>WR</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>IO/M</t>
+  </si>
+  <si>
+    <t>READY</t>
+  </si>
+  <si>
+    <t>RESET IN</t>
+  </si>
+  <si>
+    <t>CLK (OUT)</t>
+  </si>
+  <si>
+    <t>HLDA</t>
+  </si>
+  <si>
+    <t>HOLD</t>
+  </si>
+  <si>
+    <t>DM74LS12N</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>2C</t>
+  </si>
+  <si>
+    <t>2Y</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>3C</t>
+  </si>
+  <si>
+    <t>3Y</t>
+  </si>
+  <si>
+    <t>1Y</t>
+  </si>
+  <si>
+    <t>1C</t>
   </si>
 </sst>
 </file>
@@ -552,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -569,105 +716,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -685,10 +740,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1008,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792A77A1-CAB3-42EF-A3C7-FE95F01F4B1A}">
-  <dimension ref="A1:V74"/>
+  <dimension ref="A1:AP79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M84" sqref="M84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2386,28 +2437,28 @@
       <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="38">
+      <c r="C29" s="2">
         <v>0.99852724594992603</v>
       </c>
-      <c r="D29" s="38">
+      <c r="D29" s="2">
         <v>0.99852724594992603</v>
       </c>
-      <c r="E29" s="38">
+      <c r="E29" s="2">
         <v>0</v>
       </c>
-      <c r="F29" s="38">
+      <c r="F29" s="2">
         <v>0.99852724594992603</v>
       </c>
-      <c r="G29" s="38">
+      <c r="G29" s="2">
         <v>1</v>
       </c>
-      <c r="H29" s="38">
+      <c r="H29" s="2">
         <v>0.93078055964653905</v>
       </c>
-      <c r="I29" s="38">
+      <c r="I29" s="2">
         <v>0.91458026509572898</v>
       </c>
-      <c r="J29" s="38">
+      <c r="J29" s="2">
         <v>0.79970544918998498</v>
       </c>
       <c r="K29" s="1"/>
@@ -2680,1392 +2731,2079 @@
       <c r="V34" s="2"/>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="1">
         <v>16</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G36" s="10" t="s">
+      <c r="G36" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H36" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I36" s="8" t="s">
+      <c r="I36" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J36" s="6" t="s">
+      <c r="J36" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K36" s="6" t="s">
+      <c r="K36" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="L36" s="6" t="s">
+      <c r="L36" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="M36" s="6" t="s">
+      <c r="M36" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="N36" s="9" t="s">
+      <c r="N36" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="O36" s="6" t="s">
+      <c r="O36" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="P36" s="6" t="s">
+      <c r="P36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="Q36" s="6" t="s">
+      <c r="Q36" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="R36" s="6" t="s">
+      <c r="R36" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1">
         <v>1</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="1">
         <v>2</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="1">
         <v>3</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="1">
         <v>4</v>
       </c>
-      <c r="G37" s="6">
+      <c r="G37" s="1">
         <v>5</v>
       </c>
-      <c r="H37" s="6">
+      <c r="H37" s="1">
         <v>6</v>
       </c>
-      <c r="I37" s="6">
+      <c r="I37" s="1">
         <v>7</v>
       </c>
-      <c r="J37" s="6">
+      <c r="J37" s="1">
         <v>8</v>
       </c>
-      <c r="K37" s="6">
+      <c r="K37" s="1">
         <v>9</v>
       </c>
-      <c r="L37" s="6">
+      <c r="L37" s="1">
         <v>10</v>
       </c>
-      <c r="M37" s="6">
+      <c r="M37" s="1">
         <v>11</v>
       </c>
-      <c r="N37" s="6">
+      <c r="N37" s="1">
         <v>12</v>
       </c>
-      <c r="O37" s="6">
+      <c r="O37" s="1">
         <v>13</v>
       </c>
-      <c r="P37" s="6">
+      <c r="P37" s="1">
         <v>14</v>
       </c>
-      <c r="Q37" s="6">
+      <c r="Q37" s="1">
         <v>15</v>
       </c>
-      <c r="R37" s="6">
+      <c r="R37" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6" t="s">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="1">
         <v>0.66400000000000003</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="1">
         <v>0.67100000000000004</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="1">
         <v>0.64900000000000002</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="1">
         <v>0.65700000000000003</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="1">
         <v>0.63100000000000001</v>
       </c>
-      <c r="H38" s="6">
+      <c r="H38" s="1">
         <v>0.64800000000000002</v>
       </c>
-      <c r="I38" s="6">
+      <c r="I38" s="1">
         <v>0</v>
       </c>
-      <c r="J38" s="6">
+      <c r="J38" s="1">
         <v>0.61699999999999999</v>
       </c>
-      <c r="K38" s="6">
+      <c r="K38" s="1">
         <v>0.64500000000000002</v>
       </c>
-      <c r="L38" s="6">
+      <c r="L38" s="1">
         <v>0.61399999999999999</v>
       </c>
-      <c r="M38" s="6">
+      <c r="M38" s="1">
         <v>0.60499999999999998</v>
       </c>
-      <c r="N38" s="6">
+      <c r="N38" s="1">
         <v>0.627</v>
       </c>
-      <c r="O38" s="6">
+      <c r="O38" s="1">
         <v>0.66200000000000003</v>
       </c>
-      <c r="P38" s="6">
+      <c r="P38" s="1">
         <v>0.60899999999999999</v>
       </c>
-      <c r="Q38" s="6">
+      <c r="Q38" s="1">
         <v>0.66200000000000003</v>
       </c>
-      <c r="R38" s="6">
+      <c r="R38" s="1">
         <v>0.65500000000000003</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6" t="s">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="2">
         <v>0.98956780923994003</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="2">
         <v>1</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="2">
         <v>0.96721311475409799</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="2">
         <v>0.97913561847988095</v>
       </c>
-      <c r="G39" s="7">
+      <c r="G39" s="2">
         <v>0.94038748137108796</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H39" s="2">
         <v>0.965722801788376</v>
       </c>
-      <c r="I39" s="7">
+      <c r="I39" s="2">
         <v>0</v>
       </c>
-      <c r="J39" s="7">
+      <c r="J39" s="2">
         <v>0.91952309985096903</v>
       </c>
-      <c r="K39" s="7">
+      <c r="K39" s="2">
         <v>0.96125186289120701</v>
       </c>
-      <c r="L39" s="7">
+      <c r="L39" s="2">
         <v>0.91505216095380004</v>
       </c>
-      <c r="M39" s="7">
+      <c r="M39" s="2">
         <v>0.90163934426229497</v>
       </c>
-      <c r="N39" s="7">
+      <c r="N39" s="2">
         <v>0.93442622950819698</v>
       </c>
-      <c r="O39" s="7">
+      <c r="O39" s="2">
         <v>0.98658718330849504</v>
       </c>
-      <c r="P39" s="7">
+      <c r="P39" s="2">
         <v>0.90760059612518595</v>
       </c>
-      <c r="Q39" s="7">
+      <c r="Q39" s="2">
         <v>0.98658718330849504</v>
       </c>
-      <c r="R39" s="7">
+      <c r="R39" s="2">
         <v>0.97615499254843496</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
+      <c r="A40" s="1"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41" s="1">
         <v>16</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G41" s="16" t="s">
+      <c r="G41" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H41" s="12" t="s">
+      <c r="H41" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I41" s="16" t="s">
+      <c r="I41" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="J41" s="14" t="s">
+      <c r="J41" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K41" s="16" t="s">
+      <c r="K41" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="L41" s="16" t="s">
+      <c r="L41" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="M41" s="12" t="s">
+      <c r="M41" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="N41" s="12" t="s">
+      <c r="N41" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O41" s="12" t="s">
+      <c r="O41" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="P41" s="12" t="s">
+      <c r="P41" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="Q41" s="12" t="s">
+      <c r="Q41" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="R41" s="15" t="s">
+      <c r="R41" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1">
         <v>1</v>
       </c>
-      <c r="D42" s="12">
+      <c r="D42" s="1">
         <v>2</v>
       </c>
-      <c r="E42" s="12">
+      <c r="E42" s="1">
         <v>3</v>
       </c>
-      <c r="F42" s="12">
+      <c r="F42" s="1">
         <v>4</v>
       </c>
-      <c r="G42" s="12">
+      <c r="G42" s="1">
         <v>5</v>
       </c>
-      <c r="H42" s="12">
+      <c r="H42" s="1">
         <v>6</v>
       </c>
-      <c r="I42" s="12">
+      <c r="I42" s="1">
         <v>7</v>
       </c>
-      <c r="J42" s="12">
+      <c r="J42" s="1">
         <v>8</v>
       </c>
-      <c r="K42" s="12">
+      <c r="K42" s="1">
         <v>9</v>
       </c>
-      <c r="L42" s="12">
+      <c r="L42" s="1">
         <v>10</v>
       </c>
-      <c r="M42" s="12">
+      <c r="M42" s="1">
         <v>11</v>
       </c>
-      <c r="N42" s="12">
+      <c r="N42" s="1">
         <v>12</v>
       </c>
-      <c r="O42" s="12">
+      <c r="O42" s="1">
         <v>13</v>
       </c>
-      <c r="P42" s="12">
+      <c r="P42" s="1">
         <v>14</v>
       </c>
-      <c r="Q42" s="12">
+      <c r="Q42" s="1">
         <v>15</v>
       </c>
-      <c r="R42" s="12">
+      <c r="R42" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12" t="s">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C43" s="1">
         <v>0.72</v>
       </c>
-      <c r="D43" s="12">
+      <c r="D43" s="1">
         <v>0.86</v>
       </c>
-      <c r="E43" s="12">
+      <c r="E43" s="1">
         <v>0.72399999999999998</v>
       </c>
-      <c r="F43" s="12">
+      <c r="F43" s="1">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G43" s="12">
+      <c r="G43" s="1">
         <v>0.86199999999999999</v>
       </c>
-      <c r="H43" s="12">
+      <c r="H43" s="1">
         <v>0.72599999999999998</v>
       </c>
-      <c r="I43" s="12">
+      <c r="I43" s="1">
         <v>0.73099999999999998</v>
       </c>
-      <c r="J43" s="12">
+      <c r="J43" s="1">
         <v>0</v>
       </c>
-      <c r="K43" s="12">
+      <c r="K43" s="1">
         <v>0.73199999999999998</v>
       </c>
-      <c r="L43" s="12">
+      <c r="L43" s="1">
         <v>0.65</v>
       </c>
-      <c r="M43" s="12">
+      <c r="M43" s="1">
         <v>0.66800000000000004</v>
       </c>
-      <c r="N43" s="12">
+      <c r="N43" s="1">
         <v>0.65500000000000003</v>
       </c>
-      <c r="O43" s="12">
+      <c r="O43" s="1">
         <v>0.64900000000000002</v>
       </c>
-      <c r="P43" s="12">
+      <c r="P43" s="1">
         <v>0.85799999999999998</v>
       </c>
-      <c r="Q43" s="12">
+      <c r="Q43" s="1">
         <v>0.86</v>
       </c>
-      <c r="R43" s="12">
+      <c r="R43" s="1">
         <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12" t="s">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="13">
+      <c r="C44" s="2">
         <v>0.83526682134570795</v>
       </c>
-      <c r="D44" s="13">
+      <c r="D44" s="2">
         <v>0.99767981438515096</v>
       </c>
-      <c r="E44" s="13">
+      <c r="E44" s="2">
         <v>0.83990719257540603</v>
       </c>
-      <c r="F44" s="13">
+      <c r="F44" s="2">
         <v>0.83990719257540603</v>
       </c>
-      <c r="G44" s="13">
+      <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="H44" s="13">
+      <c r="H44" s="2">
         <v>0.84222737819025495</v>
       </c>
-      <c r="I44" s="13">
+      <c r="I44" s="2">
         <v>0.84802784222737804</v>
       </c>
-      <c r="J44" s="13">
+      <c r="J44" s="2">
         <v>0</v>
       </c>
-      <c r="K44" s="13">
+      <c r="K44" s="2">
         <v>0.84918793503480305</v>
       </c>
-      <c r="L44" s="13">
+      <c r="L44" s="2">
         <v>0.75406032482598595</v>
       </c>
-      <c r="M44" s="13">
+      <c r="M44" s="2">
         <v>0.77494199535962904</v>
       </c>
-      <c r="N44" s="13">
+      <c r="N44" s="2">
         <v>0.75986078886310904</v>
       </c>
-      <c r="O44" s="13">
+      <c r="O44" s="2">
         <v>0.75290023201856104</v>
       </c>
-      <c r="P44" s="13">
+      <c r="P44" s="2">
         <v>0.99535962877030204</v>
       </c>
-      <c r="Q44" s="13">
+      <c r="Q44" s="2">
         <v>0.99767981438515096</v>
       </c>
-      <c r="R44" s="13">
+      <c r="R44" s="2">
         <v>0.63805104408352697</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B46" s="17">
+      <c r="B46" s="1">
         <v>16</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D46" s="17" t="s">
+      <c r="D46" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E46" s="17" t="s">
+      <c r="E46" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F46" s="17" t="s">
+      <c r="F46" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G46" s="20" t="s">
+      <c r="G46" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H46" s="19" t="s">
+      <c r="H46" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I46" s="17" t="s">
+      <c r="I46" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J46" s="17" t="s">
+      <c r="J46" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="K46" s="17" t="s">
+      <c r="K46" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="L46" s="17" t="s">
+      <c r="L46" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="M46" s="17" t="s">
+      <c r="M46" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="N46" s="17" t="s">
+      <c r="N46" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="O46" s="17" t="s">
+      <c r="O46" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="P46" s="17" t="s">
+      <c r="P46" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="Q46" s="17" t="s">
+      <c r="Q46" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="R46" s="17" t="s">
+      <c r="R46" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1">
         <v>1</v>
       </c>
-      <c r="D47" s="17">
+      <c r="D47" s="1">
         <v>2</v>
       </c>
-      <c r="E47" s="17">
+      <c r="E47" s="1">
         <v>3</v>
       </c>
-      <c r="F47" s="17">
+      <c r="F47" s="1">
         <v>4</v>
       </c>
-      <c r="G47" s="17">
+      <c r="G47" s="1">
         <v>5</v>
       </c>
-      <c r="H47" s="17">
+      <c r="H47" s="1">
         <v>6</v>
       </c>
-      <c r="I47" s="17">
+      <c r="I47" s="1">
         <v>7</v>
       </c>
-      <c r="J47" s="17">
+      <c r="J47" s="1">
         <v>8</v>
       </c>
-      <c r="K47" s="17">
+      <c r="K47" s="1">
         <v>9</v>
       </c>
-      <c r="L47" s="17">
+      <c r="L47" s="1">
         <v>10</v>
       </c>
-      <c r="M47" s="17">
+      <c r="M47" s="1">
         <v>11</v>
       </c>
-      <c r="N47" s="17">
+      <c r="N47" s="1">
         <v>12</v>
       </c>
-      <c r="O47" s="17">
+      <c r="O47" s="1">
         <v>13</v>
       </c>
-      <c r="P47" s="17">
+      <c r="P47" s="1">
         <v>14</v>
       </c>
-      <c r="Q47" s="17">
+      <c r="Q47" s="1">
         <v>15</v>
       </c>
-      <c r="R47" s="17">
+      <c r="R47" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17" t="s">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="17">
+      <c r="C48" s="1">
         <v>0.61799999999999999</v>
       </c>
-      <c r="D48" s="17">
+      <c r="D48" s="1">
         <v>0.71599999999999997</v>
       </c>
-      <c r="E48" s="17">
+      <c r="E48" s="1">
         <v>0.76200000000000001</v>
       </c>
-      <c r="F48" s="17">
+      <c r="F48" s="1">
         <v>0.72</v>
       </c>
-      <c r="G48" s="17">
+      <c r="G48" s="1">
         <v>0.74</v>
       </c>
-      <c r="H48" s="17">
+      <c r="H48" s="1">
         <v>0</v>
       </c>
-      <c r="I48" s="17">
+      <c r="I48" s="1">
         <v>0.52400000000000002</v>
       </c>
-      <c r="J48" s="17">
+      <c r="J48" s="1">
         <v>0.76</v>
       </c>
-      <c r="K48" s="17">
+      <c r="K48" s="1">
         <v>0.66400000000000003</v>
       </c>
-      <c r="L48" s="17">
+      <c r="L48" s="1">
         <v>0.628</v>
       </c>
-      <c r="M48" s="17">
+      <c r="M48" s="1">
         <v>0.65300000000000002</v>
       </c>
-      <c r="N48" s="17">
+      <c r="N48" s="1">
         <v>0.72</v>
       </c>
-      <c r="O48" s="17">
+      <c r="O48" s="1">
         <v>0.71699999999999997</v>
       </c>
-      <c r="P48" s="17">
+      <c r="P48" s="1">
         <v>0.61499999999999999</v>
       </c>
-      <c r="Q48" s="17">
+      <c r="Q48" s="1">
         <v>0.66600000000000004</v>
       </c>
-      <c r="R48" s="17">
+      <c r="R48" s="1">
         <v>0.61799999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-      <c r="B49" s="17" t="s">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="18">
+      <c r="C49" s="2">
         <v>0.81102362204724399</v>
       </c>
-      <c r="D49" s="18">
+      <c r="D49" s="2">
         <v>0.93963254593175805</v>
       </c>
-      <c r="E49" s="18">
+      <c r="E49" s="2">
         <v>1</v>
       </c>
-      <c r="F49" s="18">
+      <c r="F49" s="2">
         <v>0.94488188976377996</v>
       </c>
-      <c r="G49" s="18">
+      <c r="G49" s="2">
         <v>0.97112860892388497</v>
       </c>
-      <c r="H49" s="18">
+      <c r="H49" s="2">
         <v>0</v>
       </c>
-      <c r="I49" s="18">
+      <c r="I49" s="2">
         <v>0.68766404199475095</v>
       </c>
-      <c r="J49" s="18">
+      <c r="J49" s="2">
         <v>0.99737532808398999</v>
       </c>
-      <c r="K49" s="18">
+      <c r="K49" s="2">
         <v>0.87139107611548605</v>
       </c>
-      <c r="L49" s="18">
+      <c r="L49" s="2">
         <v>0.82414698162729705</v>
       </c>
-      <c r="M49" s="18">
+      <c r="M49" s="2">
         <v>0.85695538057742804</v>
       </c>
-      <c r="N49" s="18">
+      <c r="N49" s="2">
         <v>0.94488188976377996</v>
       </c>
-      <c r="O49" s="18">
+      <c r="O49" s="2">
         <v>0.940944881889764</v>
       </c>
-      <c r="P49" s="18">
+      <c r="P49" s="2">
         <v>0.80708661417322802</v>
       </c>
-      <c r="Q49" s="18">
+      <c r="Q49" s="2">
         <v>0.87401574803149595</v>
       </c>
-      <c r="R49" s="18">
+      <c r="R49" s="2">
         <v>0.81102362204724399</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="22" t="s">
+      <c r="A51" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="22">
+      <c r="B51" s="1">
         <v>16</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="C51" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D51" s="22" t="s">
+      <c r="D51" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E51" s="22" t="s">
+      <c r="E51" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F51" s="22" t="s">
+      <c r="F51" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G51" s="26" t="s">
+      <c r="G51" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="H51" s="22" t="s">
+      <c r="H51" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I51" s="26" t="s">
+      <c r="I51" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="J51" s="21" t="s">
+      <c r="J51" t="s">
         <v>93</v>
       </c>
-      <c r="K51" s="21" t="s">
+      <c r="K51" t="s">
         <v>93</v>
       </c>
-      <c r="L51" s="24" t="s">
+      <c r="L51" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="M51" s="25" t="s">
+      <c r="M51" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N51" s="22" t="s">
+      <c r="N51" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="O51" s="22" t="s">
+      <c r="O51" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P51" s="22" t="s">
+      <c r="P51" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Q51" s="22"/>
-      <c r="R51" s="11"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="6"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="22">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1">
         <v>1</v>
       </c>
-      <c r="D52" s="22">
+      <c r="D52" s="1">
         <v>2</v>
       </c>
-      <c r="E52" s="22">
+      <c r="E52" s="1">
         <v>3</v>
       </c>
-      <c r="F52" s="22">
+      <c r="F52" s="1">
         <v>4</v>
       </c>
-      <c r="G52" s="22">
+      <c r="G52" s="1">
         <v>5</v>
       </c>
-      <c r="H52" s="22">
+      <c r="H52" s="1">
         <v>6</v>
       </c>
-      <c r="I52" s="22">
+      <c r="I52" s="1">
         <v>7</v>
       </c>
-      <c r="J52" s="22">
+      <c r="J52" s="1">
         <v>8</v>
       </c>
-      <c r="K52" s="22">
+      <c r="K52" s="1">
         <v>9</v>
       </c>
-      <c r="L52" s="22">
+      <c r="L52" s="1">
         <v>10</v>
       </c>
-      <c r="M52" s="22">
+      <c r="M52" s="1">
         <v>11</v>
       </c>
-      <c r="N52" s="22">
+      <c r="N52" s="1">
         <v>12</v>
       </c>
-      <c r="O52" s="22">
+      <c r="O52" s="1">
         <v>13</v>
       </c>
-      <c r="P52" s="22">
+      <c r="P52" s="1">
         <v>14</v>
       </c>
-      <c r="Q52" s="22"/>
+      <c r="Q52" s="1"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="22" t="s">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C53" s="22">
+      <c r="C53" s="1">
         <v>0.84499999999999997</v>
       </c>
-      <c r="D53" s="22">
+      <c r="D53" s="1">
         <v>0</v>
       </c>
-      <c r="E53" s="22">
+      <c r="E53" s="1">
         <v>1.89</v>
       </c>
-      <c r="F53" s="27">
+      <c r="F53" s="7">
         <v>1.9119999999999999</v>
       </c>
-      <c r="G53" s="22">
+      <c r="G53" s="1">
         <v>1.702</v>
       </c>
-      <c r="H53" s="22">
+      <c r="H53" s="1">
         <v>1.915</v>
       </c>
-      <c r="I53" s="22">
+      <c r="I53" s="1">
         <v>1.8919999999999999</v>
       </c>
-      <c r="J53" s="22">
+      <c r="J53" s="1">
         <v>1.9259999999999999</v>
       </c>
-      <c r="K53" s="22">
+      <c r="K53" s="1">
         <v>0</v>
       </c>
-      <c r="L53" s="22">
+      <c r="L53" s="1">
         <v>0</v>
       </c>
-      <c r="M53" s="22">
+      <c r="M53" s="1">
         <v>0.54</v>
       </c>
-      <c r="N53" s="22">
+      <c r="N53" s="1">
         <v>1.97</v>
       </c>
-      <c r="O53" s="22">
+      <c r="O53" s="1">
         <v>1.978</v>
       </c>
-      <c r="P53" s="22">
+      <c r="P53" s="1">
         <v>1.9730000000000001</v>
       </c>
-      <c r="Q53" s="22"/>
-      <c r="R53" s="22"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="22"/>
-      <c r="B54" s="22" t="s">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="23">
+      <c r="C54" s="2">
         <v>0.42719919110212301</v>
       </c>
-      <c r="D54" s="23">
+      <c r="D54" s="2">
         <v>0</v>
       </c>
-      <c r="E54" s="23">
+      <c r="E54" s="2">
         <v>0.95551061678463101</v>
       </c>
-      <c r="F54" s="23">
+      <c r="F54" s="2">
         <v>0.96663296258847298</v>
       </c>
-      <c r="G54" s="23">
+      <c r="G54" s="2">
         <v>0.86046511627906996</v>
       </c>
-      <c r="H54" s="23">
+      <c r="H54" s="2">
         <v>0.96814964610717902</v>
       </c>
-      <c r="I54" s="23">
+      <c r="I54" s="2">
         <v>0.95652173913043503</v>
       </c>
-      <c r="J54" s="23">
+      <c r="J54" s="2">
         <v>0.97371081900909995</v>
       </c>
-      <c r="K54" s="23">
+      <c r="K54" s="2">
         <v>0</v>
       </c>
-      <c r="L54" s="23">
+      <c r="L54" s="2">
         <v>0</v>
       </c>
-      <c r="M54" s="23">
+      <c r="M54" s="2">
         <v>0.27300303336703702</v>
       </c>
-      <c r="N54" s="23">
+      <c r="N54" s="2">
         <v>0.995955510616785</v>
       </c>
-      <c r="O54" s="23">
+      <c r="O54" s="2">
         <v>1</v>
       </c>
-      <c r="P54" s="23">
+      <c r="P54" s="2">
         <v>0.99747219413549004</v>
       </c>
-      <c r="Q54" s="22"/>
-      <c r="R54" s="22"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B56" s="29">
+      <c r="B56" s="1">
         <v>16</v>
       </c>
-      <c r="C56" s="29" t="s">
+      <c r="C56" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D56" s="29" t="s">
+      <c r="D56" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E56" s="29" t="s">
+      <c r="E56" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F56" s="29" t="s">
+      <c r="F56" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G56" s="29" t="s">
+      <c r="G56" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H56" s="29" t="s">
+      <c r="H56" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="I56" s="29" t="s">
+      <c r="I56" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J56" s="29" t="s">
+      <c r="J56" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="K56" s="31" t="s">
+      <c r="K56" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L56" s="29" t="s">
+      <c r="L56" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="M56" s="29" t="s">
+      <c r="M56" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="N56" s="29" t="s">
+      <c r="N56" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="O56" s="29" t="s">
+      <c r="O56" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="P56" s="29" t="s">
+      <c r="P56" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="Q56" s="29" t="s">
+      <c r="Q56" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="R56" s="32" t="s">
+      <c r="R56" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="29"/>
-      <c r="B57" s="29"/>
-      <c r="C57" s="29">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1">
         <v>1</v>
       </c>
-      <c r="D57" s="29">
+      <c r="D57" s="1">
         <v>2</v>
       </c>
-      <c r="E57" s="29">
+      <c r="E57" s="1">
         <v>3</v>
       </c>
-      <c r="F57" s="29">
+      <c r="F57" s="1">
         <v>4</v>
       </c>
-      <c r="G57" s="29">
+      <c r="G57" s="1">
         <v>5</v>
       </c>
-      <c r="H57" s="29">
+      <c r="H57" s="1">
         <v>6</v>
       </c>
-      <c r="I57" s="29">
+      <c r="I57" s="1">
         <v>7</v>
       </c>
-      <c r="J57" s="29">
+      <c r="J57" s="1">
         <v>8</v>
       </c>
-      <c r="K57" s="29">
+      <c r="K57" s="1">
         <v>9</v>
       </c>
-      <c r="L57" s="29">
+      <c r="L57" s="1">
         <v>10</v>
       </c>
-      <c r="M57" s="29">
+      <c r="M57" s="1">
         <v>11</v>
       </c>
-      <c r="N57" s="29">
+      <c r="N57" s="1">
         <v>12</v>
       </c>
-      <c r="O57" s="29">
+      <c r="O57" s="1">
         <v>13</v>
       </c>
-      <c r="P57" s="29">
+      <c r="P57" s="1">
         <v>14</v>
       </c>
-      <c r="Q57" s="29">
+      <c r="Q57" s="1">
         <v>15</v>
       </c>
-      <c r="R57" s="29">
+      <c r="R57" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="29"/>
-      <c r="B58" s="29" t="s">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C58" s="29">
+      <c r="C58" s="1">
         <v>0.61299999999999999</v>
       </c>
-      <c r="D58" s="29">
+      <c r="D58" s="1">
         <v>0.57199999999999995</v>
       </c>
-      <c r="E58" s="29">
+      <c r="E58" s="1">
         <v>0.57299999999999995</v>
       </c>
-      <c r="F58" s="29">
+      <c r="F58" s="1">
         <v>0.61199999999999999</v>
       </c>
-      <c r="G58" s="29">
+      <c r="G58" s="1">
         <v>0.68200000000000005</v>
       </c>
-      <c r="H58" s="29">
+      <c r="H58" s="1">
         <v>0.61</v>
       </c>
-      <c r="I58" s="29">
+      <c r="I58" s="1">
         <v>0.68200000000000005</v>
       </c>
-      <c r="J58" s="29">
+      <c r="J58" s="1">
         <v>0.61099999999999999</v>
       </c>
-      <c r="K58" s="29">
+      <c r="K58" s="1">
         <v>0</v>
       </c>
-      <c r="L58" s="29">
+      <c r="L58" s="1">
         <v>0.61199999999999999</v>
       </c>
-      <c r="M58" s="29">
+      <c r="M58" s="1">
         <v>0.68200000000000005</v>
       </c>
-      <c r="N58" s="29">
+      <c r="N58" s="1">
         <v>0.64400000000000002</v>
       </c>
-      <c r="O58" s="29">
+      <c r="O58" s="1">
         <v>0.61199999999999999</v>
       </c>
-      <c r="P58" s="29">
+      <c r="P58" s="1">
         <v>0.54</v>
       </c>
-      <c r="Q58" s="29">
+      <c r="Q58" s="1">
         <v>0.63600000000000001</v>
       </c>
-      <c r="R58" s="29">
+      <c r="R58" s="1">
         <v>0.58299999999999996</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="29"/>
-      <c r="B59" s="29" t="s">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C59" s="30">
+      <c r="C59" s="2">
         <v>0.89882697947214096</v>
       </c>
-      <c r="D59" s="30">
+      <c r="D59" s="2">
         <v>0.83870967741935498</v>
       </c>
-      <c r="E59" s="30">
+      <c r="E59" s="2">
         <v>0.84017595307917903</v>
       </c>
-      <c r="F59" s="30">
+      <c r="F59" s="2">
         <v>0.89736070381231703</v>
       </c>
-      <c r="G59" s="30">
+      <c r="G59" s="2">
         <v>1</v>
       </c>
-      <c r="H59" s="30">
+      <c r="H59" s="2">
         <v>0.89442815249266805</v>
       </c>
-      <c r="I59" s="30">
+      <c r="I59" s="2">
         <v>1</v>
       </c>
-      <c r="J59" s="30">
+      <c r="J59" s="2">
         <v>0.89589442815249298</v>
       </c>
-      <c r="K59" s="30">
+      <c r="K59" s="2">
         <v>0</v>
       </c>
-      <c r="L59" s="30">
+      <c r="L59" s="2">
         <v>0.89736070381231703</v>
       </c>
-      <c r="M59" s="30">
+      <c r="M59" s="2">
         <v>1</v>
       </c>
-      <c r="N59" s="30">
+      <c r="N59" s="2">
         <v>0.94428152492668604</v>
       </c>
-      <c r="O59" s="30">
+      <c r="O59" s="2">
         <v>0.89736070381231703</v>
       </c>
-      <c r="P59" s="30">
+      <c r="P59" s="2">
         <v>0.79178885630498497</v>
       </c>
-      <c r="Q59" s="30">
+      <c r="Q59" s="2">
         <v>0.93255131964809401</v>
       </c>
-      <c r="R59" s="30">
+      <c r="R59" s="2">
         <v>0.85483870967741904</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
+      <c r="A61" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B61" s="33">
+      <c r="B61" s="1">
         <v>8</v>
       </c>
-      <c r="C61" s="33" t="s">
+      <c r="C61" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D61" s="36" t="s">
+      <c r="D61" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E61" s="35" t="s">
+      <c r="E61" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F61" s="33" t="s">
+      <c r="F61" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G61" s="33" t="s">
+      <c r="G61" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H61" s="33" t="s">
+      <c r="H61" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="I61" s="33" t="s">
+      <c r="I61" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="J61" s="33" t="s">
+      <c r="J61" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="K61" s="28"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="33"/>
-      <c r="B62" s="33"/>
-      <c r="C62" s="33">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1">
         <v>1</v>
       </c>
-      <c r="D62" s="33">
+      <c r="D62" s="1">
         <v>2</v>
       </c>
-      <c r="E62" s="33">
+      <c r="E62" s="1">
         <v>3</v>
       </c>
-      <c r="F62" s="33">
+      <c r="F62" s="1">
         <v>4</v>
       </c>
-      <c r="G62" s="33">
+      <c r="G62" s="1">
         <v>5</v>
       </c>
-      <c r="H62" s="33">
+      <c r="H62" s="1">
         <v>6</v>
       </c>
-      <c r="I62" s="33">
+      <c r="I62" s="1">
         <v>7</v>
       </c>
-      <c r="J62" s="33">
+      <c r="J62" s="1">
         <v>8</v>
       </c>
-      <c r="K62" s="28"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A63" s="33"/>
-      <c r="B63" s="33" t="s">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="33">
+      <c r="C63" s="1">
         <v>0.60799999999999998</v>
       </c>
-      <c r="D63" s="33">
+      <c r="D63" s="1">
         <v>0.58799999999999997</v>
       </c>
-      <c r="E63" s="33">
+      <c r="E63" s="1">
         <v>0</v>
       </c>
-      <c r="F63" s="33">
+      <c r="F63" s="1">
         <v>0.60899999999999999</v>
       </c>
-      <c r="G63" s="33">
+      <c r="G63" s="1">
         <v>0</v>
       </c>
-      <c r="H63" s="33">
+      <c r="H63" s="1">
         <v>1.1459999999999999</v>
       </c>
-      <c r="I63" s="33">
+      <c r="I63" s="1">
         <v>1.1459999999999999</v>
       </c>
-      <c r="J63" s="33">
+      <c r="J63" s="1">
         <v>1.147</v>
       </c>
-      <c r="K63" s="29"/>
+      <c r="K63" s="1"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A64" s="33"/>
-      <c r="B64" s="33" t="s">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C64" s="34">
+      <c r="C64" s="2">
         <v>0.53007846556233695</v>
       </c>
-      <c r="D64" s="34">
+      <c r="D64" s="2">
         <v>0.512641673931996</v>
       </c>
-      <c r="E64" s="34">
+      <c r="E64" s="2">
         <v>0</v>
       </c>
-      <c r="F64" s="34">
+      <c r="F64" s="2">
         <v>0.530950305143854</v>
       </c>
-      <c r="G64" s="34">
+      <c r="G64" s="2">
         <v>0</v>
       </c>
-      <c r="H64" s="34">
+      <c r="H64" s="2">
         <v>0.99912816041848296</v>
       </c>
-      <c r="I64" s="34">
+      <c r="I64" s="2">
         <v>0.99912816041848296</v>
       </c>
-      <c r="J64" s="34">
+      <c r="J64" s="2">
         <v>1</v>
       </c>
-      <c r="K64" s="28"/>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K65" s="28"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" s="37" t="s">
+    </row>
+    <row r="66" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="37">
+      <c r="B66" s="1">
         <v>16</v>
       </c>
-      <c r="C66" s="37" t="s">
+      <c r="C66" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D66" s="37" t="s">
+      <c r="D66" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E66" s="37" t="s">
+      <c r="E66" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F66" s="37" t="s">
+      <c r="F66" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G66" s="37" t="s">
+      <c r="G66" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H66" s="37" t="s">
+      <c r="H66" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I66" s="37" t="s">
+      <c r="I66" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J66" s="39" t="s">
+      <c r="J66" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="K66" s="37" t="s">
+      <c r="K66" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="L66" s="37" t="s">
+      <c r="L66" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="M66" s="37" t="s">
+      <c r="M66" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="N66" s="37" t="s">
+      <c r="N66" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O66" s="37" t="s">
+      <c r="O66" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="P66" s="40" t="s">
+      <c r="P66" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A67" s="37"/>
-      <c r="B67" s="37"/>
-      <c r="C67" s="37">
+    <row r="67" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1">
         <v>1</v>
       </c>
-      <c r="D67" s="37">
+      <c r="D67" s="1">
         <v>2</v>
       </c>
-      <c r="E67" s="37">
+      <c r="E67" s="1">
         <v>3</v>
       </c>
-      <c r="F67" s="37">
+      <c r="F67" s="1">
         <v>4</v>
       </c>
-      <c r="G67" s="37">
+      <c r="G67" s="1">
         <v>5</v>
       </c>
-      <c r="H67" s="37">
+      <c r="H67" s="1">
         <v>6</v>
       </c>
-      <c r="I67" s="37">
+      <c r="I67" s="1">
         <v>7</v>
       </c>
-      <c r="J67" s="37">
+      <c r="J67" s="1">
         <v>8</v>
       </c>
-      <c r="K67" s="37">
+      <c r="K67" s="1">
         <v>9</v>
       </c>
-      <c r="L67" s="37">
+      <c r="L67" s="1">
         <v>10</v>
       </c>
-      <c r="M67" s="37">
+      <c r="M67" s="1">
         <v>11</v>
       </c>
-      <c r="N67" s="37">
+      <c r="N67" s="1">
         <v>12</v>
       </c>
-      <c r="O67" s="37">
+      <c r="O67" s="1">
         <v>13</v>
       </c>
-      <c r="P67" s="37">
+      <c r="P67" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A68" s="37"/>
-      <c r="B68" s="37" t="s">
+    <row r="68" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C68" s="37">
+      <c r="C68" s="1">
         <v>1.6779999999999999</v>
       </c>
-      <c r="D68" s="37">
+      <c r="D68" s="1">
         <v>1.6970000000000001</v>
       </c>
-      <c r="E68" s="37">
+      <c r="E68" s="1">
         <v>0.67500000000000004</v>
       </c>
-      <c r="F68" s="37">
+      <c r="F68" s="1">
         <v>1.72</v>
       </c>
-      <c r="G68" s="37">
+      <c r="G68" s="1">
         <v>0.67200000000000004</v>
       </c>
-      <c r="H68" s="37">
+      <c r="H68" s="1">
         <v>1.7050000000000001</v>
       </c>
-      <c r="I68" s="37">
+      <c r="I68" s="1">
         <v>0</v>
       </c>
-      <c r="J68" s="37">
+      <c r="J68" s="1">
         <v>1.6879999999999999</v>
       </c>
-      <c r="K68" s="37">
+      <c r="K68" s="1">
         <v>0.67200000000000004</v>
       </c>
-      <c r="L68" s="37">
+      <c r="L68" s="1">
         <v>0.67200000000000004</v>
       </c>
-      <c r="M68" s="37">
+      <c r="M68" s="1">
         <v>0.67100000000000004</v>
       </c>
-      <c r="N68" s="37">
+      <c r="N68" s="1">
         <v>1.6950000000000001</v>
       </c>
-      <c r="O68" s="37">
+      <c r="O68" s="1">
         <v>1.6819999999999999</v>
       </c>
-      <c r="P68" s="37">
+      <c r="P68" s="1">
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69" s="37"/>
-      <c r="B69" s="37" t="s">
+    <row r="69" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C69" s="38">
+      <c r="C69" s="2">
         <v>0.97558139534883703</v>
       </c>
-      <c r="D69" s="38">
+      <c r="D69" s="2">
         <v>0.98662790697674396</v>
       </c>
-      <c r="E69" s="38">
+      <c r="E69" s="2">
         <v>0.39244186046511598</v>
       </c>
-      <c r="F69" s="38">
+      <c r="F69" s="2">
         <v>1</v>
       </c>
-      <c r="G69" s="38">
+      <c r="G69" s="2">
         <v>0.39069767441860498</v>
       </c>
-      <c r="H69" s="38">
+      <c r="H69" s="2">
         <v>0.99127906976744196</v>
       </c>
-      <c r="I69" s="38">
+      <c r="I69" s="2">
         <v>0</v>
       </c>
-      <c r="J69" s="38">
+      <c r="J69" s="2">
         <v>0.98139534883720903</v>
       </c>
-      <c r="K69" s="38">
+      <c r="K69" s="2">
         <v>0.39069767441860498</v>
       </c>
-      <c r="L69" s="38">
+      <c r="L69" s="2">
         <v>0.39069767441860498</v>
       </c>
-      <c r="M69" s="38">
+      <c r="M69" s="2">
         <v>0.39011627906976698</v>
       </c>
-      <c r="N69" s="38">
+      <c r="N69" s="2">
         <v>0.98546511627906996</v>
       </c>
-      <c r="O69" s="38">
+      <c r="O69" s="2">
         <v>0.97790697674418603</v>
       </c>
-      <c r="P69" s="38">
+      <c r="P69" s="2">
         <v>0.34360465116279099</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A74" s="37"/>
+    <row r="71" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" s="1">
+        <v>40</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="M71" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="N71" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="O71" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P71" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q71" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="R71" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="S71" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="T71" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="U71" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="V71" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="W71" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="X71" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y71" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z71" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AA71" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB71" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC71" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD71" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE71" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF71" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AG71" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="AH71" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="AI71" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="AJ71" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="AK71" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="AL71" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="AM71" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AN71" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AO71" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AP71" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1">
+        <v>1</v>
+      </c>
+      <c r="D72" s="1">
+        <v>2</v>
+      </c>
+      <c r="E72" s="1">
+        <v>3</v>
+      </c>
+      <c r="F72" s="1">
+        <v>4</v>
+      </c>
+      <c r="G72" s="1">
+        <v>5</v>
+      </c>
+      <c r="H72" s="1">
+        <v>6</v>
+      </c>
+      <c r="I72" s="1">
+        <v>7</v>
+      </c>
+      <c r="J72" s="1">
+        <v>8</v>
+      </c>
+      <c r="K72" s="1">
+        <v>9</v>
+      </c>
+      <c r="L72" s="1">
+        <v>10</v>
+      </c>
+      <c r="M72" s="1">
+        <v>11</v>
+      </c>
+      <c r="N72" s="1">
+        <v>12</v>
+      </c>
+      <c r="O72" s="1">
+        <v>13</v>
+      </c>
+      <c r="P72" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q72" s="1">
+        <v>15</v>
+      </c>
+      <c r="R72" s="1">
+        <v>16</v>
+      </c>
+      <c r="S72" s="1">
+        <v>17</v>
+      </c>
+      <c r="T72" s="1">
+        <v>18</v>
+      </c>
+      <c r="U72" s="1">
+        <v>19</v>
+      </c>
+      <c r="V72" s="1">
+        <v>20</v>
+      </c>
+      <c r="W72" s="1">
+        <v>21</v>
+      </c>
+      <c r="X72" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y72" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z72" s="1">
+        <v>24</v>
+      </c>
+      <c r="AA72" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB72" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC72" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD72" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE72" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF72" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG72" s="1">
+        <v>31</v>
+      </c>
+      <c r="AH72" s="1">
+        <v>32</v>
+      </c>
+      <c r="AI72" s="1">
+        <v>33</v>
+      </c>
+      <c r="AJ72" s="1">
+        <v>34</v>
+      </c>
+      <c r="AK72" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL72" s="1">
+        <v>36</v>
+      </c>
+      <c r="AM72" s="1">
+        <v>37</v>
+      </c>
+      <c r="AN72" s="1">
+        <v>38</v>
+      </c>
+      <c r="AO72" s="1">
+        <v>39</v>
+      </c>
+      <c r="AP72" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1.4550000000000001</v>
+      </c>
+      <c r="D73" s="1">
+        <v>1.163</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1.202</v>
+      </c>
+      <c r="F73" s="1">
+        <v>1.198</v>
+      </c>
+      <c r="G73" s="1">
+        <v>1.4510000000000001</v>
+      </c>
+      <c r="H73" s="1">
+        <v>1.4490000000000001</v>
+      </c>
+      <c r="I73" s="1">
+        <v>1.448</v>
+      </c>
+      <c r="J73" s="1">
+        <v>1.4450000000000001</v>
+      </c>
+      <c r="K73" s="1">
+        <v>1.4470000000000001</v>
+      </c>
+      <c r="L73" s="1">
+        <v>1.478</v>
+      </c>
+      <c r="M73" s="1">
+        <v>1.2110000000000001</v>
+      </c>
+      <c r="N73" s="1">
+        <v>1.21</v>
+      </c>
+      <c r="O73" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="P73" s="1">
+        <v>1.2829999999999999</v>
+      </c>
+      <c r="Q73" s="1">
+        <v>1.234</v>
+      </c>
+      <c r="R73" s="1">
+        <v>1.4970000000000001</v>
+      </c>
+      <c r="S73" s="1">
+        <v>1.5429999999999999</v>
+      </c>
+      <c r="T73" s="1">
+        <v>1.5449999999999999</v>
+      </c>
+      <c r="U73" s="1">
+        <v>1.5609999999999999</v>
+      </c>
+      <c r="V73" s="1">
+        <v>0</v>
+      </c>
+      <c r="W73" s="1">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="X73" s="1">
+        <v>1.4419999999999999</v>
+      </c>
+      <c r="Y73" s="1">
+        <v>1.248</v>
+      </c>
+      <c r="Z73" s="1">
+        <v>1.333</v>
+      </c>
+      <c r="AA73" s="1">
+        <v>1.4430000000000001</v>
+      </c>
+      <c r="AB73" s="1">
+        <v>1.448</v>
+      </c>
+      <c r="AC73" s="1">
+        <v>1.3779999999999999</v>
+      </c>
+      <c r="AD73" s="1">
+        <v>1.357</v>
+      </c>
+      <c r="AE73" s="1">
+        <v>1.38</v>
+      </c>
+      <c r="AF73" s="1">
+        <v>1.357</v>
+      </c>
+      <c r="AG73" s="1">
+        <v>1.42</v>
+      </c>
+      <c r="AH73" s="1">
+        <v>1.665</v>
+      </c>
+      <c r="AI73" s="1">
+        <v>1.5489999999999999</v>
+      </c>
+      <c r="AJ73" s="1">
+        <v>1.262</v>
+      </c>
+      <c r="AK73" s="1">
+        <v>1.3280000000000001</v>
+      </c>
+      <c r="AL73" s="1">
+        <v>1.2829999999999999</v>
+      </c>
+      <c r="AM73" s="1">
+        <v>1.29</v>
+      </c>
+      <c r="AN73" s="1">
+        <v>1.254</v>
+      </c>
+      <c r="AO73" s="1">
+        <v>1.492</v>
+      </c>
+      <c r="AP73" s="1">
+        <v>1.423</v>
+      </c>
+    </row>
+    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0.87387387387387405</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0.69849849849849899</v>
+      </c>
+      <c r="E74" s="1">
+        <v>0.72192192192192195</v>
+      </c>
+      <c r="F74" s="1">
+        <v>0.71951951951951898</v>
+      </c>
+      <c r="G74" s="1">
+        <v>0.87147147147147197</v>
+      </c>
+      <c r="H74" s="1">
+        <v>0.87027027027027004</v>
+      </c>
+      <c r="I74" s="1">
+        <v>0.86966966966966996</v>
+      </c>
+      <c r="J74" s="1">
+        <v>0.86786786786786796</v>
+      </c>
+      <c r="K74" s="1">
+        <v>0.869069069069069</v>
+      </c>
+      <c r="L74" s="1">
+        <v>0.88768768768768802</v>
+      </c>
+      <c r="M74" s="1">
+        <v>0.72732732732732697</v>
+      </c>
+      <c r="N74" s="1">
+        <v>0.726726726726727</v>
+      </c>
+      <c r="O74" s="1">
+        <v>0.73873873873873896</v>
+      </c>
+      <c r="P74" s="1">
+        <v>0.77057057057057099</v>
+      </c>
+      <c r="Q74" s="1">
+        <v>0.74114114114114105</v>
+      </c>
+      <c r="R74" s="1">
+        <v>0.89909909909909902</v>
+      </c>
+      <c r="S74" s="1">
+        <v>0.92672672672672696</v>
+      </c>
+      <c r="T74" s="1">
+        <v>0.927927927927928</v>
+      </c>
+      <c r="U74" s="1">
+        <v>0.93753753753753699</v>
+      </c>
+      <c r="V74" s="1">
+        <v>0</v>
+      </c>
+      <c r="W74" s="1">
+        <v>0.55435435435435398</v>
+      </c>
+      <c r="X74" s="1">
+        <v>0.86606606606606595</v>
+      </c>
+      <c r="Y74" s="1">
+        <v>0.74954954954955</v>
+      </c>
+      <c r="Z74" s="1">
+        <v>0.80060060060060101</v>
+      </c>
+      <c r="AA74" s="1">
+        <v>0.86666666666666703</v>
+      </c>
+      <c r="AB74" s="1">
+        <v>0.86966966966966996</v>
+      </c>
+      <c r="AC74" s="1">
+        <v>0.82762762762762798</v>
+      </c>
+      <c r="AD74" s="1">
+        <v>0.81501501501501505</v>
+      </c>
+      <c r="AE74" s="1">
+        <v>0.82882882882882902</v>
+      </c>
+      <c r="AF74" s="1">
+        <v>0.81501501501501505</v>
+      </c>
+      <c r="AG74" s="1">
+        <v>0.85285285285285295</v>
+      </c>
+      <c r="AH74" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI74" s="1">
+        <v>0.93033033033032997</v>
+      </c>
+      <c r="AJ74" s="1">
+        <v>0.75795795795795795</v>
+      </c>
+      <c r="AK74" s="1">
+        <v>0.79759759759759796</v>
+      </c>
+      <c r="AL74" s="1">
+        <v>0.77057057057057099</v>
+      </c>
+      <c r="AM74" s="1">
+        <v>0.77477477477477497</v>
+      </c>
+      <c r="AN74" s="1">
+        <v>0.75315315315315301</v>
+      </c>
+      <c r="AO74" s="1">
+        <v>0.89609609609609597</v>
+      </c>
+      <c r="AP74" s="1">
+        <v>0.85465465465465495</v>
+      </c>
+    </row>
+    <row r="76" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B76" s="1">
+        <v>14</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="N76" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="O76" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="P76" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1">
+        <v>1</v>
+      </c>
+      <c r="D77" s="1">
+        <v>2</v>
+      </c>
+      <c r="E77" s="1">
+        <v>3</v>
+      </c>
+      <c r="F77" s="1">
+        <v>4</v>
+      </c>
+      <c r="G77" s="1">
+        <v>5</v>
+      </c>
+      <c r="H77" s="1">
+        <v>6</v>
+      </c>
+      <c r="I77" s="1">
+        <v>7</v>
+      </c>
+      <c r="J77" s="1">
+        <v>8</v>
+      </c>
+      <c r="K77" s="1">
+        <v>9</v>
+      </c>
+      <c r="L77" s="1">
+        <v>10</v>
+      </c>
+      <c r="M77" s="1">
+        <v>11</v>
+      </c>
+      <c r="N77" s="1">
+        <v>12</v>
+      </c>
+      <c r="O77" s="1">
+        <v>13</v>
+      </c>
+      <c r="P77" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="F78" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G78" s="1">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="H78" s="1">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="I78" s="1">
+        <v>0</v>
+      </c>
+      <c r="J78" s="1">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="K78" s="1">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="L78" s="1">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="M78" s="1">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="N78" s="1">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="O78" s="1">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="P78" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="79" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79" s="1">
+        <v>0.85007727975270497</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0.83771251931993795</v>
+      </c>
+      <c r="E79" s="1">
+        <v>0.85162287480680099</v>
+      </c>
+      <c r="F79" s="1">
+        <v>0.85007727975270497</v>
+      </c>
+      <c r="G79" s="1">
+        <v>0.84544049459041704</v>
+      </c>
+      <c r="H79" s="1">
+        <v>0.99690880989180797</v>
+      </c>
+      <c r="I79" s="1">
+        <v>0</v>
+      </c>
+      <c r="J79" s="1">
+        <v>0.99227202472952103</v>
+      </c>
+      <c r="K79" s="1">
+        <v>0.85935085007727996</v>
+      </c>
+      <c r="L79" s="1">
+        <v>0.84544049459041704</v>
+      </c>
+      <c r="M79" s="1">
+        <v>0.842349304482226</v>
+      </c>
+      <c r="N79" s="1">
+        <v>1</v>
+      </c>
+      <c r="O79" s="1">
+        <v>0.84389489953632202</v>
+      </c>
+      <c r="P79" s="1">
+        <v>0.88098918083462097</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>